<commit_message>
First sentences in intro and discussion
</commit_message>
<xml_diff>
--- a/results/glms results/bWP GLMs.xlsx
+++ b/results/glms results/bWP GLMs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Hidro_thermal_experiments/results/glms results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{D2949686-EA14-4584-BCBB-B509E8615AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{999D7E9B-6660-4EB0-AADD-5CB515B09853}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{D2949686-EA14-4584-BCBB-B509E8615AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5763FCF-428B-4A68-A4BD-C38B95DF7B0F}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F79B5BD8-CE6D-4DD7-A183-E06843C689D4}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F79B5BD8-CE6D-4DD7-A183-E06843C689D4}"/>
   </bookViews>
   <sheets>
     <sheet name="both sowing" sheetId="1" r:id="rId1"/>
@@ -218,10 +218,10 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -405,9 +405,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -445,7 +445,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -551,7 +551,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -693,7 +693,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D348CBC9-CCB0-4FDF-9DB5-ECC7C87690DA}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:F43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129326FF-5BB7-4F2B-A111-E14CC6228B87}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:F42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,7 +1175,7 @@
         <v>1.3640000000000001</v>
       </c>
       <c r="E21">
-        <v>0.1724</v>
+        <v>0.18940000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC79FD1B-B94F-4B32-9EA7-B7EC02A35F1A}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21:F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>